<commit_message>
right graph for 10gbps, in rack, even, striping
</commit_message>
<xml_diff>
--- a/distributed-tensorflow-simulator/exp_results/inception-v3/graphs/10gbps_inrack_even_striping.xlsx
+++ b/distributed-tensorflow-simulator/exp_results/inception-v3/graphs/10gbps_inrack_even_striping.xlsx
@@ -14,9 +14,6 @@
   <sheets>
     <sheet name="out" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -264,16 +261,16 @@
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>2.4138</c:v>
+                    <c:v>3.2836</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>4.6919</c:v>
+                    <c:v>4.5183</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>3.0454</c:v>
+                    <c:v>4.592</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>2.1509</c:v>
+                    <c:v>3.2224</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -285,19 +282,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>1.0897</c:v>
+                    <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.1514</c:v>
+                    <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>6.0497</c:v>
+                    <c:v>4.7777</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.9792</c:v>
+                    <c:v>13.7478</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>1.1329</c:v>
+                    <c:v>7.8521</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -350,16 +347,16 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-1.1342</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15.1841</c:v>
+                  <c:v>16.0954</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>29.1862</c:v>
+                  <c:v>27.939</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>36.1446</c:v>
+                  <c:v>35.7378</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -408,19 +405,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.388</c:v>
+                    <c:v>0.2237</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.0779</c:v>
+                    <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.7056</c:v>
+                    <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>3.3229</c:v>
+                    <c:v>1.1591</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>3.0211</c:v>
+                    <c:v>1.5003</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -432,19 +429,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.2804</c:v>
+                    <c:v>0.321</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.6254</c:v>
+                    <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.4523</c:v>
+                    <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>53.4639</c:v>
+                    <c:v>19.8974</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>15.0049</c:v>
+                    <c:v>3.2224</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -494,19 +491,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0.1311</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-1.1026</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11.9737</c:v>
+                  <c:v>12.3434</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>28.7461</c:v>
+                  <c:v>28.5383</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -555,19 +552,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.1704</c:v>
+                    <c:v>0.1645</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.427</c:v>
+                    <c:v>0.3052</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.3422</c:v>
+                    <c:v>0.0349</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>34.6339</c:v>
+                    <c:v>5.7256</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>9.5602</c:v>
+                    <c:v>23.2817</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -579,19 +576,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.1704</c:v>
+                    <c:v>0.2028</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.3837</c:v>
+                    <c:v>0.3272</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.8165</c:v>
+                    <c:v>0.0349</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>96.4694</c:v>
+                    <c:v>6.1184</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>4.5371</c:v>
+                    <c:v>16.4774</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -644,16 +641,16 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.1788</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.2783</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.6706</c:v>
+                  <c:v>-5.1959</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>17.8096</c:v>
+                  <c:v>12.6687</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -702,19 +699,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0312</c:v>
+                    <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0376</c:v>
+                    <c:v>0.0382</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.276</c:v>
+                    <c:v>0.1761</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>28.6096</c:v>
+                    <c:v>15.0781</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>4.9889</c:v>
+                    <c:v>4.2495</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -729,16 +726,16 @@
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.036</c:v>
+                    <c:v>0.0381</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.2508</c:v>
+                    <c:v>0.3554</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>9.0695</c:v>
+                    <c:v>21.9474</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>15.9682</c:v>
+                    <c:v>6.5054</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -794,13 +791,13 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0178</c:v>
+                  <c:v>0.0327</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-3.2829</c:v>
+                  <c:v>0.3044</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.8222</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -815,11 +812,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2078507088"/>
-        <c:axId val="-2077809952"/>
+        <c:axId val="-2130673312"/>
+        <c:axId val="-2129925952"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2078507088"/>
+        <c:axId val="-2130673312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -936,12 +933,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2077809952"/>
+        <c:crossAx val="-2129925952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2077809952"/>
+        <c:axId val="-2129925952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1071,7 +1068,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2078507088"/>
+        <c:crossAx val="-2130673312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1293,19 +1290,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.6512</c:v>
+                    <c:v>0.4963</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.188</c:v>
+                    <c:v>0.1687</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.7213</c:v>
+                    <c:v>0.7364</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.7269</c:v>
+                    <c:v>1.0751</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.2998</c:v>
+                    <c:v>1.5076</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1317,19 +1314,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>2.4194</c:v>
+                    <c:v>1.0506</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.1179</c:v>
+                    <c:v>2.4275</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.4019</c:v>
+                    <c:v>0.6871</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.7284</c:v>
+                    <c:v>1.8164</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.982</c:v>
+                    <c:v>1.3624</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1379,19 +1376,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>12.8273</c:v>
+                  <c:v>8.393</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.9829</c:v>
+                  <c:v>21.5364</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>29.3004</c:v>
+                  <c:v>32.3275</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40.2494</c:v>
+                  <c:v>42.2368</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>45.32</c:v>
+                  <c:v>46.3246</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1440,19 +1437,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0342</c:v>
+                    <c:v>0.1242</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.9642</c:v>
+                    <c:v>0.4003</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.3593</c:v>
+                    <c:v>1.2435</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.0457</c:v>
+                    <c:v>0.7969</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>1.489</c:v>
+                    <c:v>0.4541</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1464,19 +1461,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.4776</c:v>
+                    <c:v>0.2558</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.9991</c:v>
+                    <c:v>1.0987</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.6714</c:v>
+                    <c:v>1.2093</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>2.1677</c:v>
+                    <c:v>1.1846</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>1.6043</c:v>
+                    <c:v>1.1007</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1526,19 +1523,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.5866</c:v>
+                  <c:v>0.5407</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12.8473</c:v>
+                  <c:v>8.4076</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.0357</c:v>
+                  <c:v>20.2929</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>29.6491</c:v>
+                  <c:v>32.7746</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40.6025</c:v>
+                  <c:v>42.2794</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1587,19 +1584,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.1704</c:v>
+                    <c:v>0.1645</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.2594</c:v>
+                    <c:v>0.3066</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.0414</c:v>
+                    <c:v>0.5923</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>27.3871</c:v>
+                    <c:v>5.9654</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>10.8069</c:v>
+                    <c:v>20.138</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1614,16 +1611,16 @@
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.1701</c:v>
+                    <c:v>0.1704</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.9778</c:v>
+                    <c:v>0.5348</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>67.1795</c:v>
+                    <c:v>8.3424</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.9707</c:v>
+                    <c:v>39.6279</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1676,16 +1673,16 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.3576</c:v>
+                  <c:v>0.3228</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12.0568</c:v>
+                  <c:v>7.8326</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14.6069</c:v>
+                  <c:v>18.1687</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>30.726</c:v>
+                  <c:v>33.0685</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1734,19 +1731,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0312</c:v>
+                    <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0376</c:v>
+                    <c:v>0.0382</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.0835</c:v>
+                    <c:v>0.0827</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>21.0994</c:v>
+                    <c:v>12.7484</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>1.6553</c:v>
+                    <c:v>14.423</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1764,13 +1761,13 @@
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.2031</c:v>
+                    <c:v>0.126</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>32.4923</c:v>
+                    <c:v>11.5727</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>48.4588</c:v>
+                    <c:v>40.3893</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1826,13 +1823,13 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.303</c:v>
+                  <c:v>0.2779</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.2736</c:v>
+                  <c:v>7.1679</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.8152</c:v>
+                  <c:v>9.5865</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1847,11 +1844,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2089053616"/>
-        <c:axId val="-2089097056"/>
+        <c:axId val="-2130328848"/>
+        <c:axId val="-2130242464"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2089053616"/>
+        <c:axId val="-2130328848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1968,12 +1965,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2089097056"/>
+        <c:crossAx val="-2130242464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2089097056"/>
+        <c:axId val="-2130242464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2103,7 +2100,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2089053616"/>
+        <c:crossAx val="-2130328848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2325,19 +2322,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.6512</c:v>
+                    <c:v>0.4963</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.4316</c:v>
+                    <c:v>3.4201</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>4.3249</c:v>
+                    <c:v>4.3523</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.2551</c:v>
+                    <c:v>2.0858</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.8771</c:v>
+                    <c:v>0.2852</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2349,19 +2346,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>2.4194</c:v>
+                    <c:v>1.0506</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>2.1669</c:v>
+                    <c:v>2.4597</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>4.756</c:v>
+                    <c:v>4.5739</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>17.0229</c:v>
+                    <c:v>6.7464</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>9.2752</c:v>
+                    <c:v>5.3591</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2411,19 +2408,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>12.8273</c:v>
+                  <c:v>8.393</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.0583</c:v>
+                  <c:v>21.5686</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>48.7055</c:v>
+                  <c:v>51.5535</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>72.5393</c:v>
+                  <c:v>74.5479</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>86.2028</c:v>
+                  <c:v>86.942</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2472,19 +2469,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0342</c:v>
+                    <c:v>0.1242</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.9642</c:v>
+                    <c:v>0.4003</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.3593</c:v>
+                    <c:v>1.2435</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>6.5768</c:v>
+                    <c:v>5.8077</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>4.4716</c:v>
+                    <c:v>3.8603</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2496,19 +2493,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.4776</c:v>
+                    <c:v>0.2558</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.9991</c:v>
+                    <c:v>1.0987</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.6714</c:v>
+                    <c:v>1.2093</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>9.3845</c:v>
+                    <c:v>57.675</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>15.7714</c:v>
+                    <c:v>2.5278</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2558,19 +2555,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.5866</c:v>
+                  <c:v>0.5407</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12.8473</c:v>
+                  <c:v>8.4076</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.0357</c:v>
+                  <c:v>20.2929</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>45.3056</c:v>
+                  <c:v>48.5443</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>70.6268</c:v>
+                  <c:v>70.8689</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2619,19 +2616,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.1704</c:v>
+                    <c:v>0.1645</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.2594</c:v>
+                    <c:v>0.3066</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.0414</c:v>
+                    <c:v>0.5923</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>36.6684</c:v>
+                    <c:v>5.2432</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>1.3361</c:v>
+                    <c:v>14.9735</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2646,16 +2643,16 @@
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.1701</c:v>
+                    <c:v>0.1704</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.9778</c:v>
+                    <c:v>0.5348</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>53.5785</c:v>
+                    <c:v>9.5306</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>22.1802</c:v>
+                    <c:v>7.6049</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2708,16 +2705,16 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.3576</c:v>
+                  <c:v>0.3228</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12.0568</c:v>
+                  <c:v>7.8326</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.3059</c:v>
+                  <c:v>19.1089</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>46.2134</c:v>
+                  <c:v>49.1341</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2766,19 +2763,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0312</c:v>
+                    <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0376</c:v>
+                    <c:v>0.0382</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.0835</c:v>
+                    <c:v>0.0827</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>11.8713</c:v>
+                    <c:v>16.9773</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>8.0533</c:v>
+                    <c:v>6.1828</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2796,13 +2793,13 @@
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.2031</c:v>
+                    <c:v>0.126</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>9.3425</c:v>
+                    <c:v>10.6864</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>23.888</c:v>
+                    <c:v>52.0765</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2858,13 +2855,13 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.303</c:v>
+                  <c:v>0.2779</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.3232</c:v>
+                  <c:v>7.4836</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.164</c:v>
+                  <c:v>18.7608</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2879,11 +2876,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2089471136"/>
-        <c:axId val="-2089268048"/>
+        <c:axId val="-2130121504"/>
+        <c:axId val="-2119899920"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2089471136"/>
+        <c:axId val="-2130121504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3000,12 +2997,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2089268048"/>
+        <c:crossAx val="-2119899920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2089268048"/>
+        <c:axId val="-2119899920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3135,7 +3132,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2089471136"/>
+        <c:crossAx val="-2130121504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3357,19 +3354,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0</c:v>
+                    <c:v>0.0202</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>3.9343</c:v>
+                    <c:v>4.1939</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>6.6866</c:v>
+                    <c:v>6.9352</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>3.5115</c:v>
+                    <c:v>4.8255</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>1.7282</c:v>
+                    <c:v>0.2817</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3387,13 +3384,13 @@
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>7.1654</c:v>
+                    <c:v>7.465</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>29.1501</c:v>
+                    <c:v>10.5065</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>16.9108</c:v>
+                    <c:v>10.2199</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3449,13 +3446,13 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>27.0684</c:v>
+                  <c:v>28.2545</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>53.8632</c:v>
+                  <c:v>55.698</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>74.7155</c:v>
+                  <c:v>75.67230000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3513,10 +3510,10 @@
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>7.4372</c:v>
+                    <c:v>9.1937</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>7.5614</c:v>
+                    <c:v>6.5885</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3537,10 +3534,10 @@
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>14.0051</c:v>
+                    <c:v>88.226</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>29.1534</c:v>
+                    <c:v>4.7501</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3599,10 +3596,10 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23.3563</c:v>
+                  <c:v>23.943</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>51.1949</c:v>
+                  <c:v>49.4689</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3660,10 +3657,10 @@
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>48.452</c:v>
+                    <c:v>10.6247</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>2.7579</c:v>
+                    <c:v>25.549</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3684,10 +3681,10 @@
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>52.4369</c:v>
+                    <c:v>11.869</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>51.3226</c:v>
+                    <c:v>12.5705</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3746,10 +3743,10 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-7.3788</c:v>
+                  <c:v>-0.3306</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>21.3918</c:v>
+                  <c:v>23.9117</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3807,10 +3804,10 @@
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>27.7247</c:v>
+                    <c:v>3.8459</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>17.5414</c:v>
+                    <c:v>11.9122</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3831,10 +3828,10 @@
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>12.2411</c:v>
+                    <c:v>14.0095</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>12.4666</c:v>
+                    <c:v>17.4629</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3893,10 +3890,10 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.7736</c:v>
+                  <c:v>7.541</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.3038</c:v>
+                  <c:v>6.7545</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3911,11 +3908,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2079852112"/>
-        <c:axId val="-2078775776"/>
+        <c:axId val="-2088466960"/>
+        <c:axId val="-2088460736"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2079852112"/>
+        <c:axId val="-2088466960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4032,12 +4029,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2078775776"/>
+        <c:crossAx val="-2088460736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2078775776"/>
+        <c:axId val="-2088460736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4167,7 +4164,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2079852112"/>
+        <c:crossAx val="-2088466960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6609,915 +6606,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="out"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="4">
-          <cell r="D4">
-            <v>2</v>
-          </cell>
-          <cell r="E4">
-            <v>0</v>
-          </cell>
-          <cell r="F4">
-            <v>1.0911999999999999</v>
-          </cell>
-          <cell r="G4">
-            <v>1.0779000000000001</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="D5">
-            <v>4</v>
-          </cell>
-          <cell r="E5">
-            <v>1.2456</v>
-          </cell>
-          <cell r="F5">
-            <v>1.407</v>
-          </cell>
-          <cell r="G5">
-            <v>0.99739999999999995</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="D6">
-            <v>8</v>
-          </cell>
-          <cell r="E6">
-            <v>16.129000000000001</v>
-          </cell>
-          <cell r="F6">
-            <v>3.9912999999999998</v>
-          </cell>
-          <cell r="G6">
-            <v>4.5518999999999998</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="D7">
-            <v>16</v>
-          </cell>
-          <cell r="E7">
-            <v>28.493200000000002</v>
-          </cell>
-          <cell r="F7">
-            <v>12.5747</v>
-          </cell>
-          <cell r="G7">
-            <v>2.8045</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="D8">
-            <v>32</v>
-          </cell>
-          <cell r="E8">
-            <v>36.925699999999999</v>
-          </cell>
-          <cell r="F8">
-            <v>7.7286999999999999</v>
-          </cell>
-          <cell r="G8">
-            <v>1.1873</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="E10">
-            <v>0</v>
-          </cell>
-          <cell r="F10">
-            <v>0</v>
-          </cell>
-          <cell r="G10">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="E11">
-            <v>0</v>
-          </cell>
-          <cell r="F11">
-            <v>0</v>
-          </cell>
-          <cell r="G11">
-            <v>3.3603000000000001</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="E12">
-            <v>17.674199999999999</v>
-          </cell>
-          <cell r="F12">
-            <v>4.8032000000000004</v>
-          </cell>
-          <cell r="G12">
-            <v>4.5731999999999999</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="E13">
-            <v>29.992100000000001</v>
-          </cell>
-          <cell r="F13">
-            <v>26.671199999999999</v>
-          </cell>
-          <cell r="G13">
-            <v>2.1979000000000002</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="E14">
-            <v>37.325299999999999</v>
-          </cell>
-          <cell r="F14">
-            <v>3.5363000000000002</v>
-          </cell>
-          <cell r="G14">
-            <v>0.55710000000000004</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="E16">
-            <v>0</v>
-          </cell>
-          <cell r="F16">
-            <v>0</v>
-          </cell>
-          <cell r="G16">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="E17">
-            <v>0</v>
-          </cell>
-          <cell r="F17">
-            <v>2.0400000000000001E-2</v>
-          </cell>
-          <cell r="G17">
-            <v>2.0500000000000001E-2</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="E18">
-            <v>0</v>
-          </cell>
-          <cell r="F18">
-            <v>0</v>
-          </cell>
-          <cell r="G18">
-            <v>7.585</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="E19">
-            <v>18.0519</v>
-          </cell>
-          <cell r="F19">
-            <v>1.6042000000000001</v>
-          </cell>
-          <cell r="G19">
-            <v>3.2688999999999999</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="E20">
-            <v>32.878100000000003</v>
-          </cell>
-          <cell r="F20">
-            <v>11.919</v>
-          </cell>
-          <cell r="G20">
-            <v>2.7446000000000002</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="E22">
-            <v>0</v>
-          </cell>
-          <cell r="F22">
-            <v>0.3196</v>
-          </cell>
-          <cell r="G22">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="E23">
-            <v>0</v>
-          </cell>
-          <cell r="F23">
-            <v>0</v>
-          </cell>
-          <cell r="G23">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="E24">
-            <v>0</v>
-          </cell>
-          <cell r="F24">
-            <v>0</v>
-          </cell>
-          <cell r="G24">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="E25">
-            <v>-1.3866000000000001</v>
-          </cell>
-          <cell r="F25">
-            <v>9.5091000000000001</v>
-          </cell>
-          <cell r="G25">
-            <v>13.7889</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="E26">
-            <v>20.470700000000001</v>
-          </cell>
-          <cell r="F26">
-            <v>44.099600000000002</v>
-          </cell>
-          <cell r="G26">
-            <v>15.2531</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="E29">
-            <v>11.7545</v>
-          </cell>
-          <cell r="F29">
-            <v>1.3320000000000001</v>
-          </cell>
-          <cell r="G29">
-            <v>1.724</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="E30">
-            <v>9.9132999999999996</v>
-          </cell>
-          <cell r="F30">
-            <v>1.7428999999999999</v>
-          </cell>
-          <cell r="G30">
-            <v>1.355</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="E31">
-            <v>29.48</v>
-          </cell>
-          <cell r="F31">
-            <v>0.44230000000000003</v>
-          </cell>
-          <cell r="G31">
-            <v>0.60260000000000002</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="E32">
-            <v>39.526699999999998</v>
-          </cell>
-          <cell r="F32">
-            <v>0.69899999999999995</v>
-          </cell>
-          <cell r="G32">
-            <v>1.5249999999999999</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="E33">
-            <v>45.844299999999997</v>
-          </cell>
-          <cell r="F33">
-            <v>0.89900000000000002</v>
-          </cell>
-          <cell r="G33">
-            <v>0.51139999999999997</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="E35">
-            <v>13.3262</v>
-          </cell>
-          <cell r="F35">
-            <v>1.4916</v>
-          </cell>
-          <cell r="G35">
-            <v>0.68930000000000002</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="E36">
-            <v>13.0052</v>
-          </cell>
-          <cell r="F36">
-            <v>1.5077</v>
-          </cell>
-          <cell r="G36">
-            <v>0.1249</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="E37">
-            <v>34.027099999999997</v>
-          </cell>
-          <cell r="F37">
-            <v>0.56200000000000006</v>
-          </cell>
-          <cell r="G37">
-            <v>0.77129999999999999</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="E38">
-            <v>44.891300000000001</v>
-          </cell>
-          <cell r="F38">
-            <v>1.9685999999999999</v>
-          </cell>
-          <cell r="G38">
-            <v>0.78090000000000004</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="E39">
-            <v>49.067</v>
-          </cell>
-          <cell r="F39">
-            <v>0.48970000000000002</v>
-          </cell>
-          <cell r="G39">
-            <v>1.5214000000000001</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="E41">
-            <v>1.4333</v>
-          </cell>
-          <cell r="F41">
-            <v>0.1797</v>
-          </cell>
-          <cell r="G41">
-            <v>8.4900000000000003E-2</v>
-          </cell>
-        </row>
-        <row r="42">
-          <cell r="E42">
-            <v>-14.854100000000001</v>
-          </cell>
-          <cell r="F42">
-            <v>0.83220000000000005</v>
-          </cell>
-          <cell r="G42">
-            <v>2.2370000000000001</v>
-          </cell>
-        </row>
-        <row r="43">
-          <cell r="E43">
-            <v>15.901400000000001</v>
-          </cell>
-          <cell r="F43">
-            <v>0.60099999999999998</v>
-          </cell>
-          <cell r="G43">
-            <v>0.59899999999999998</v>
-          </cell>
-        </row>
-        <row r="44">
-          <cell r="E44">
-            <v>34.833199999999998</v>
-          </cell>
-          <cell r="F44">
-            <v>3.4192999999999998</v>
-          </cell>
-          <cell r="G44">
-            <v>0.62690000000000001</v>
-          </cell>
-        </row>
-        <row r="45">
-          <cell r="E45">
-            <v>44.505499999999998</v>
-          </cell>
-          <cell r="F45">
-            <v>0.72640000000000005</v>
-          </cell>
-          <cell r="G45">
-            <v>0.4834</v>
-          </cell>
-        </row>
-        <row r="47">
-          <cell r="E47">
-            <v>0</v>
-          </cell>
-          <cell r="F47">
-            <v>0</v>
-          </cell>
-          <cell r="G47">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="48">
-          <cell r="E48">
-            <v>2.5449999999999999</v>
-          </cell>
-          <cell r="F48">
-            <v>0.32979999999999998</v>
-          </cell>
-          <cell r="G48">
-            <v>0.12</v>
-          </cell>
-        </row>
-        <row r="49">
-          <cell r="E49">
-            <v>-10.950100000000001</v>
-          </cell>
-          <cell r="F49">
-            <v>0.89039999999999997</v>
-          </cell>
-          <cell r="G49">
-            <v>0.83489999999999998</v>
-          </cell>
-        </row>
-        <row r="50">
-          <cell r="E50">
-            <v>16.394300000000001</v>
-          </cell>
-          <cell r="F50">
-            <v>54.334499999999998</v>
-          </cell>
-          <cell r="G50">
-            <v>16.245100000000001</v>
-          </cell>
-        </row>
-        <row r="51">
-          <cell r="E51">
-            <v>36.4</v>
-          </cell>
-          <cell r="F51">
-            <v>24.002400000000002</v>
-          </cell>
-          <cell r="G51">
-            <v>13.4595</v>
-          </cell>
-        </row>
-        <row r="54">
-          <cell r="E54">
-            <v>11.7545</v>
-          </cell>
-          <cell r="F54">
-            <v>1.3320000000000001</v>
-          </cell>
-          <cell r="G54">
-            <v>1.724</v>
-          </cell>
-        </row>
-        <row r="55">
-          <cell r="E55">
-            <v>10.0258</v>
-          </cell>
-          <cell r="F55">
-            <v>1.0678000000000001</v>
-          </cell>
-          <cell r="G55">
-            <v>1.7574000000000001</v>
-          </cell>
-        </row>
-        <row r="56">
-          <cell r="E56">
-            <v>48.6616</v>
-          </cell>
-          <cell r="F56">
-            <v>4.6632999999999996</v>
-          </cell>
-          <cell r="G56">
-            <v>4.3293999999999997</v>
-          </cell>
-        </row>
-        <row r="57">
-          <cell r="E57">
-            <v>72.901899999999998</v>
-          </cell>
-          <cell r="F57">
-            <v>17.129000000000001</v>
-          </cell>
-          <cell r="G57">
-            <v>2.3666999999999998</v>
-          </cell>
-        </row>
-        <row r="58">
-          <cell r="E58">
-            <v>86.078199999999995</v>
-          </cell>
-          <cell r="F58">
-            <v>5.3712</v>
-          </cell>
-          <cell r="G58">
-            <v>1.7237</v>
-          </cell>
-        </row>
-        <row r="60">
-          <cell r="E60">
-            <v>13.3262</v>
-          </cell>
-          <cell r="F60">
-            <v>1.4916</v>
-          </cell>
-          <cell r="G60">
-            <v>0.68930000000000002</v>
-          </cell>
-        </row>
-        <row r="61">
-          <cell r="E61">
-            <v>13.0253</v>
-          </cell>
-          <cell r="F61">
-            <v>1.5278</v>
-          </cell>
-          <cell r="G61">
-            <v>3.4495</v>
-          </cell>
-        </row>
-        <row r="62">
-          <cell r="E62">
-            <v>51.950099999999999</v>
-          </cell>
-          <cell r="F62">
-            <v>4.2807000000000004</v>
-          </cell>
-          <cell r="G62">
-            <v>3.9687000000000001</v>
-          </cell>
-        </row>
-        <row r="63">
-          <cell r="E63">
-            <v>75.480199999999996</v>
-          </cell>
-          <cell r="F63">
-            <v>5.0841000000000003</v>
-          </cell>
-          <cell r="G63">
-            <v>0.93200000000000005</v>
-          </cell>
-        </row>
-        <row r="64">
-          <cell r="E64">
-            <v>87.154899999999998</v>
-          </cell>
-          <cell r="F64">
-            <v>13.6145</v>
-          </cell>
-          <cell r="G64">
-            <v>5.8700000000000002E-2</v>
-          </cell>
-        </row>
-        <row r="66">
-          <cell r="E66">
-            <v>1.4333</v>
-          </cell>
-          <cell r="F66">
-            <v>0.1797</v>
-          </cell>
-          <cell r="G66">
-            <v>8.4900000000000003E-2</v>
-          </cell>
-        </row>
-        <row r="67">
-          <cell r="E67">
-            <v>-14.854100000000001</v>
-          </cell>
-          <cell r="F67">
-            <v>0.83220000000000005</v>
-          </cell>
-          <cell r="G67">
-            <v>2.2370000000000001</v>
-          </cell>
-        </row>
-        <row r="68">
-          <cell r="E68">
-            <v>16.253599999999999</v>
-          </cell>
-          <cell r="F68">
-            <v>0.95320000000000005</v>
-          </cell>
-          <cell r="G68">
-            <v>7.2328000000000001</v>
-          </cell>
-        </row>
-        <row r="69">
-          <cell r="E69">
-            <v>54.555500000000002</v>
-          </cell>
-          <cell r="F69">
-            <v>6.726</v>
-          </cell>
-          <cell r="G69">
-            <v>3.8308</v>
-          </cell>
-        </row>
-        <row r="70">
-          <cell r="E70">
-            <v>77.211399999999998</v>
-          </cell>
-          <cell r="F70">
-            <v>2.6758999999999999</v>
-          </cell>
-          <cell r="G70">
-            <v>0.42659999999999998</v>
-          </cell>
-        </row>
-        <row r="72">
-          <cell r="E72">
-            <v>0</v>
-          </cell>
-          <cell r="F72">
-            <v>0</v>
-          </cell>
-          <cell r="G72">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="73">
-          <cell r="E73">
-            <v>2.5449999999999999</v>
-          </cell>
-          <cell r="F73">
-            <v>0.32979999999999998</v>
-          </cell>
-          <cell r="G73">
-            <v>0.12</v>
-          </cell>
-        </row>
-        <row r="74">
-          <cell r="E74">
-            <v>-10.950100000000001</v>
-          </cell>
-          <cell r="F74">
-            <v>0.89039999999999997</v>
-          </cell>
-          <cell r="G74">
-            <v>0.83489999999999998</v>
-          </cell>
-        </row>
-        <row r="75">
-          <cell r="E75">
-            <v>18.454599999999999</v>
-          </cell>
-          <cell r="F75">
-            <v>4.1291000000000002</v>
-          </cell>
-          <cell r="G75">
-            <v>10.368399999999999</v>
-          </cell>
-        </row>
-        <row r="76">
-          <cell r="E76">
-            <v>56.583799999999997</v>
-          </cell>
-          <cell r="F76">
-            <v>13.653700000000001</v>
-          </cell>
-          <cell r="G76">
-            <v>8.9168000000000003</v>
-          </cell>
-        </row>
-        <row r="79">
-          <cell r="E79">
-            <v>0</v>
-          </cell>
-          <cell r="F79">
-            <v>0</v>
-          </cell>
-          <cell r="G79">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="80">
-          <cell r="E80">
-            <v>0</v>
-          </cell>
-          <cell r="F80">
-            <v>0</v>
-          </cell>
-          <cell r="G80">
-            <v>3.9342999999999999</v>
-          </cell>
-        </row>
-        <row r="81">
-          <cell r="E81">
-            <v>27.0684</v>
-          </cell>
-          <cell r="F81">
-            <v>7.1654</v>
-          </cell>
-          <cell r="G81">
-            <v>6.6866000000000003</v>
-          </cell>
-        </row>
-        <row r="82">
-          <cell r="E82">
-            <v>55.046999999999997</v>
-          </cell>
-          <cell r="F82">
-            <v>28.687000000000001</v>
-          </cell>
-          <cell r="G82">
-            <v>4.4339000000000004</v>
-          </cell>
-        </row>
-        <row r="83">
-          <cell r="E83">
-            <v>74.048000000000002</v>
-          </cell>
-          <cell r="F83">
-            <v>9.0913000000000004</v>
-          </cell>
-          <cell r="G83">
-            <v>3.4348000000000001</v>
-          </cell>
-        </row>
-        <row r="85">
-          <cell r="E85">
-            <v>0</v>
-          </cell>
-          <cell r="F85">
-            <v>0</v>
-          </cell>
-          <cell r="G85">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="86">
-          <cell r="E86">
-            <v>0</v>
-          </cell>
-          <cell r="F86">
-            <v>0</v>
-          </cell>
-          <cell r="G86">
-            <v>3.8502999999999998</v>
-          </cell>
-        </row>
-        <row r="87">
-          <cell r="E87">
-            <v>26.8826</v>
-          </cell>
-          <cell r="F87">
-            <v>7.1422999999999996</v>
-          </cell>
-          <cell r="G87">
-            <v>6.6585999999999999</v>
-          </cell>
-        </row>
-        <row r="88">
-          <cell r="E88">
-            <v>56.129899999999999</v>
-          </cell>
-          <cell r="F88">
-            <v>8.9312000000000005</v>
-          </cell>
-          <cell r="G88">
-            <v>0.91120000000000001</v>
-          </cell>
-        </row>
-        <row r="89">
-          <cell r="E89">
-            <v>74.415499999999994</v>
-          </cell>
-          <cell r="F89">
-            <v>26.265499999999999</v>
-          </cell>
-          <cell r="G89">
-            <v>0.64980000000000004</v>
-          </cell>
-        </row>
-        <row r="91">
-          <cell r="E91">
-            <v>0</v>
-          </cell>
-          <cell r="F91">
-            <v>0</v>
-          </cell>
-          <cell r="G91">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="92">
-          <cell r="E92">
-            <v>0</v>
-          </cell>
-          <cell r="F92">
-            <v>0</v>
-          </cell>
-          <cell r="G92">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="93">
-          <cell r="E93">
-            <v>0</v>
-          </cell>
-          <cell r="F93">
-            <v>0</v>
-          </cell>
-          <cell r="G93">
-            <v>9.0191999999999997</v>
-          </cell>
-        </row>
-        <row r="94">
-          <cell r="E94">
-            <v>30.857199999999999</v>
-          </cell>
-          <cell r="F94">
-            <v>7.4958999999999998</v>
-          </cell>
-          <cell r="G94">
-            <v>4.9538000000000002</v>
-          </cell>
-        </row>
-        <row r="95">
-          <cell r="E95">
-            <v>58.700400000000002</v>
-          </cell>
-          <cell r="F95">
-            <v>3.9940000000000002</v>
-          </cell>
-          <cell r="G95">
-            <v>1.3427</v>
-          </cell>
-        </row>
-        <row r="97">
-          <cell r="E97">
-            <v>0</v>
-          </cell>
-          <cell r="F97">
-            <v>0</v>
-          </cell>
-          <cell r="G97">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="98">
-          <cell r="E98">
-            <v>0</v>
-          </cell>
-          <cell r="F98">
-            <v>0</v>
-          </cell>
-          <cell r="G98">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="99">
-          <cell r="E99">
-            <v>0</v>
-          </cell>
-          <cell r="F99">
-            <v>0</v>
-          </cell>
-          <cell r="G99">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="100">
-          <cell r="E100">
-            <v>1.8240000000000001</v>
-          </cell>
-          <cell r="F100">
-            <v>8.5667000000000009</v>
-          </cell>
-          <cell r="G100">
-            <v>38.8934</v>
-          </cell>
-        </row>
-        <row r="101">
-          <cell r="E101">
-            <v>31.768999999999998</v>
-          </cell>
-          <cell r="F101">
-            <v>21.7742</v>
-          </cell>
-          <cell r="G101">
-            <v>11.7645</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7785,8 +6873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G101"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="P24" sqref="P24"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="R21" sqref="R21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7853,7 +6941,7 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>1.0896999999999999</v>
+        <v>0</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -7873,13 +6961,13 @@
         <v>4</v>
       </c>
       <c r="E5">
-        <v>-1.1342000000000001</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <v>0.15140000000000001</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>2.4138000000000002</v>
+        <v>3.2835999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -7896,13 +6984,13 @@
         <v>8</v>
       </c>
       <c r="E6">
-        <v>15.184100000000001</v>
+        <v>16.095400000000001</v>
       </c>
       <c r="F6">
-        <v>6.0496999999999996</v>
+        <v>4.7777000000000003</v>
       </c>
       <c r="G6">
-        <v>4.6919000000000004</v>
+        <v>4.5183</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -7919,13 +7007,13 @@
         <v>16</v>
       </c>
       <c r="E7">
-        <v>29.186199999999999</v>
+        <v>27.939</v>
       </c>
       <c r="F7">
-        <v>1.9792000000000001</v>
+        <v>13.7478</v>
       </c>
       <c r="G7">
-        <v>3.0453999999999999</v>
+        <v>4.5919999999999996</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -7942,13 +7030,13 @@
         <v>32</v>
       </c>
       <c r="E8">
-        <v>36.144599999999997</v>
+        <v>35.7378</v>
       </c>
       <c r="F8">
-        <v>1.1329</v>
+        <v>7.8521000000000001</v>
       </c>
       <c r="G8">
-        <v>2.1509</v>
+        <v>3.2223999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -7965,13 +7053,13 @@
         <v>2</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>0.13109999999999999</v>
       </c>
       <c r="F10">
-        <v>0.28039999999999998</v>
+        <v>0.32100000000000001</v>
       </c>
       <c r="G10">
-        <v>0.38800000000000001</v>
+        <v>0.22370000000000001</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -7991,10 +7079,10 @@
         <v>0</v>
       </c>
       <c r="F11">
-        <v>0.62539999999999996</v>
+        <v>0</v>
       </c>
       <c r="G11">
-        <v>1.0779000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -8011,13 +7099,13 @@
         <v>8</v>
       </c>
       <c r="E12">
-        <v>-1.1026</v>
+        <v>0</v>
       </c>
       <c r="F12">
-        <v>1.4522999999999999</v>
+        <v>0</v>
       </c>
       <c r="G12">
-        <v>1.7056</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -8034,13 +7122,13 @@
         <v>16</v>
       </c>
       <c r="E13">
-        <v>11.973699999999999</v>
+        <v>12.343400000000001</v>
       </c>
       <c r="F13">
-        <v>53.463900000000002</v>
+        <v>19.897400000000001</v>
       </c>
       <c r="G13">
-        <v>3.3229000000000002</v>
+        <v>1.1591</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -8057,13 +7145,13 @@
         <v>32</v>
       </c>
       <c r="E14">
-        <v>28.746099999999998</v>
+        <v>28.5383</v>
       </c>
       <c r="F14">
-        <v>15.004899999999999</v>
+        <v>3.2223999999999999</v>
       </c>
       <c r="G14">
-        <v>3.0211000000000001</v>
+        <v>1.5003</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -8083,10 +7171,10 @@
         <v>0</v>
       </c>
       <c r="F16">
-        <v>0.1704</v>
+        <v>0.20280000000000001</v>
       </c>
       <c r="G16">
-        <v>0.1704</v>
+        <v>0.16450000000000001</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -8103,13 +7191,13 @@
         <v>4</v>
       </c>
       <c r="E17">
-        <v>-0.17879999999999999</v>
+        <v>0</v>
       </c>
       <c r="F17">
-        <v>0.38369999999999999</v>
+        <v>0.32719999999999999</v>
       </c>
       <c r="G17">
-        <v>0.42699999999999999</v>
+        <v>0.30520000000000003</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -8126,13 +7214,13 @@
         <v>8</v>
       </c>
       <c r="E18">
-        <v>0.27829999999999999</v>
+        <v>0</v>
       </c>
       <c r="F18">
-        <v>0.8165</v>
+        <v>3.49E-2</v>
       </c>
       <c r="G18">
-        <v>0.3422</v>
+        <v>3.49E-2</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -8149,13 +7237,13 @@
         <v>16</v>
       </c>
       <c r="E19">
-        <v>1.6706000000000001</v>
+        <v>-5.1959</v>
       </c>
       <c r="F19">
-        <v>96.469399999999993</v>
+        <v>6.1184000000000003</v>
       </c>
       <c r="G19">
-        <v>34.633899999999997</v>
+        <v>5.7256</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -8172,13 +7260,13 @@
         <v>32</v>
       </c>
       <c r="E20">
-        <v>17.8096</v>
+        <v>12.668699999999999</v>
       </c>
       <c r="F20">
-        <v>4.5370999999999997</v>
+        <v>16.477399999999999</v>
       </c>
       <c r="G20">
-        <v>9.5602</v>
+        <v>23.281700000000001</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -8201,7 +7289,7 @@
         <v>0</v>
       </c>
       <c r="G22">
-        <v>3.1199999999999999E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -8221,10 +7309,10 @@
         <v>0</v>
       </c>
       <c r="F23">
-        <v>3.5999999999999997E-2</v>
+        <v>3.8100000000000002E-2</v>
       </c>
       <c r="G23">
-        <v>3.7600000000000001E-2</v>
+        <v>3.8199999999999998E-2</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -8241,13 +7329,13 @@
         <v>8</v>
       </c>
       <c r="E24">
-        <v>1.78E-2</v>
+        <v>3.27E-2</v>
       </c>
       <c r="F24">
-        <v>0.25080000000000002</v>
+        <v>0.35539999999999999</v>
       </c>
       <c r="G24">
-        <v>0.27600000000000002</v>
+        <v>0.17610000000000001</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -8264,13 +7352,13 @@
         <v>16</v>
       </c>
       <c r="E25">
-        <v>-3.2829000000000002</v>
+        <v>0.3044</v>
       </c>
       <c r="F25">
-        <v>9.0694999999999997</v>
+        <v>21.947399999999998</v>
       </c>
       <c r="G25">
-        <v>28.6096</v>
+        <v>15.078099999999999</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -8287,13 +7375,13 @@
         <v>32</v>
       </c>
       <c r="E26">
-        <v>-0.82220000000000004</v>
+        <v>0</v>
       </c>
       <c r="F26">
-        <v>15.9682</v>
+        <v>6.5053999999999998</v>
       </c>
       <c r="G26">
-        <v>4.9889000000000001</v>
+        <v>4.2495000000000003</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -8318,13 +7406,13 @@
         <v>2</v>
       </c>
       <c r="E29">
-        <v>12.827299999999999</v>
+        <v>8.3930000000000007</v>
       </c>
       <c r="F29">
-        <v>2.4194</v>
+        <v>1.0506</v>
       </c>
       <c r="G29">
-        <v>0.6512</v>
+        <v>0.49630000000000002</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -8341,13 +7429,13 @@
         <v>4</v>
       </c>
       <c r="E30">
-        <v>8.9829000000000008</v>
+        <v>21.5364</v>
       </c>
       <c r="F30">
-        <v>1.1178999999999999</v>
+        <v>2.4275000000000002</v>
       </c>
       <c r="G30">
-        <v>1.1879999999999999</v>
+        <v>0.16869999999999999</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -8364,13 +7452,13 @@
         <v>8</v>
       </c>
       <c r="E31">
-        <v>29.3004</v>
+        <v>32.327500000000001</v>
       </c>
       <c r="F31">
-        <v>0.40189999999999998</v>
+        <v>0.68710000000000004</v>
       </c>
       <c r="G31">
-        <v>0.72130000000000005</v>
+        <v>0.73640000000000005</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
@@ -8387,13 +7475,13 @@
         <v>16</v>
       </c>
       <c r="E32">
-        <v>40.249400000000001</v>
+        <v>42.236800000000002</v>
       </c>
       <c r="F32">
-        <v>1.7283999999999999</v>
+        <v>1.8164</v>
       </c>
       <c r="G32">
-        <v>0.72689999999999999</v>
+        <v>1.0750999999999999</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
@@ -8410,13 +7498,13 @@
         <v>32</v>
       </c>
       <c r="E33">
-        <v>45.32</v>
+        <v>46.324599999999997</v>
       </c>
       <c r="F33">
-        <v>0.98199999999999998</v>
+        <v>1.3624000000000001</v>
       </c>
       <c r="G33">
-        <v>0.29980000000000001</v>
+        <v>1.5076000000000001</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
@@ -8433,13 +7521,13 @@
         <v>2</v>
       </c>
       <c r="E35">
-        <v>0.58660000000000001</v>
+        <v>0.54069999999999996</v>
       </c>
       <c r="F35">
-        <v>0.47760000000000002</v>
+        <v>0.25580000000000003</v>
       </c>
       <c r="G35">
-        <v>3.4200000000000001E-2</v>
+        <v>0.1242</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
@@ -8456,13 +7544,13 @@
         <v>4</v>
       </c>
       <c r="E36">
-        <v>12.847300000000001</v>
+        <v>8.4076000000000004</v>
       </c>
       <c r="F36">
-        <v>1.9991000000000001</v>
+        <v>1.0987</v>
       </c>
       <c r="G36">
-        <v>0.96419999999999995</v>
+        <v>0.40029999999999999</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
@@ -8479,13 +7567,13 @@
         <v>8</v>
       </c>
       <c r="E37">
-        <v>9.0357000000000003</v>
+        <v>20.292899999999999</v>
       </c>
       <c r="F37">
-        <v>1.6714</v>
+        <v>1.2093</v>
       </c>
       <c r="G37">
-        <v>1.3593</v>
+        <v>1.2435</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
@@ -8502,13 +7590,13 @@
         <v>16</v>
       </c>
       <c r="E38">
-        <v>29.649100000000001</v>
+        <v>32.7746</v>
       </c>
       <c r="F38">
-        <v>2.1677</v>
+        <v>1.1846000000000001</v>
       </c>
       <c r="G38">
-        <v>1.0457000000000001</v>
+        <v>0.79690000000000005</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
@@ -8525,13 +7613,13 @@
         <v>32</v>
       </c>
       <c r="E39">
-        <v>40.602499999999999</v>
+        <v>42.279400000000003</v>
       </c>
       <c r="F39">
-        <v>1.6043000000000001</v>
+        <v>1.1007</v>
       </c>
       <c r="G39">
-        <v>1.4890000000000001</v>
+        <v>0.4541</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
@@ -8554,7 +7642,7 @@
         <v>0</v>
       </c>
       <c r="G41">
-        <v>0.1704</v>
+        <v>0.16450000000000001</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
@@ -8571,13 +7659,13 @@
         <v>4</v>
       </c>
       <c r="E42">
-        <v>0.35759999999999997</v>
+        <v>0.32279999999999998</v>
       </c>
       <c r="F42">
-        <v>0.1701</v>
+        <v>0.1704</v>
       </c>
       <c r="G42">
-        <v>0.25940000000000002</v>
+        <v>0.30659999999999998</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
@@ -8594,13 +7682,13 @@
         <v>8</v>
       </c>
       <c r="E43">
-        <v>12.056800000000001</v>
+        <v>7.8326000000000002</v>
       </c>
       <c r="F43">
-        <v>0.9778</v>
+        <v>0.53480000000000005</v>
       </c>
       <c r="G43">
-        <v>1.0414000000000001</v>
+        <v>0.59230000000000005</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
@@ -8617,13 +7705,13 @@
         <v>16</v>
       </c>
       <c r="E44">
-        <v>14.6069</v>
+        <v>18.168700000000001</v>
       </c>
       <c r="F44">
-        <v>67.179500000000004</v>
+        <v>8.3423999999999996</v>
       </c>
       <c r="G44">
-        <v>27.3871</v>
+        <v>5.9653999999999998</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
@@ -8640,13 +7728,13 @@
         <v>32</v>
       </c>
       <c r="E45">
-        <v>30.725999999999999</v>
+        <v>33.0685</v>
       </c>
       <c r="F45">
-        <v>0.97070000000000001</v>
+        <v>39.627899999999997</v>
       </c>
       <c r="G45">
-        <v>10.806900000000001</v>
+        <v>20.138000000000002</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
@@ -8669,7 +7757,7 @@
         <v>0</v>
       </c>
       <c r="G47">
-        <v>3.1199999999999999E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
@@ -8692,7 +7780,7 @@
         <v>0</v>
       </c>
       <c r="G48">
-        <v>3.7600000000000001E-2</v>
+        <v>3.8199999999999998E-2</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
@@ -8709,13 +7797,13 @@
         <v>8</v>
       </c>
       <c r="E49">
-        <v>0.30299999999999999</v>
+        <v>0.27789999999999998</v>
       </c>
       <c r="F49">
-        <v>0.2031</v>
+        <v>0.126</v>
       </c>
       <c r="G49">
-        <v>8.3500000000000005E-2</v>
+        <v>8.2699999999999996E-2</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
@@ -8732,13 +7820,13 @@
         <v>16</v>
       </c>
       <c r="E50">
-        <v>4.2736000000000001</v>
+        <v>7.1679000000000004</v>
       </c>
       <c r="F50">
-        <v>32.4923</v>
+        <v>11.572699999999999</v>
       </c>
       <c r="G50">
-        <v>21.099399999999999</v>
+        <v>12.7484</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
@@ -8755,13 +7843,13 @@
         <v>32</v>
       </c>
       <c r="E51">
-        <v>8.8152000000000008</v>
+        <v>9.5864999999999991</v>
       </c>
       <c r="F51">
-        <v>48.458799999999997</v>
+        <v>40.389299999999999</v>
       </c>
       <c r="G51">
-        <v>1.6553</v>
+        <v>14.423</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
@@ -8786,13 +7874,13 @@
         <v>2</v>
       </c>
       <c r="E54">
-        <v>12.827299999999999</v>
+        <v>8.3930000000000007</v>
       </c>
       <c r="F54">
-        <v>2.4194</v>
+        <v>1.0506</v>
       </c>
       <c r="G54">
-        <v>0.6512</v>
+        <v>0.49630000000000002</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
@@ -8809,13 +7897,13 @@
         <v>4</v>
       </c>
       <c r="E55">
-        <v>10.058299999999999</v>
+        <v>21.5686</v>
       </c>
       <c r="F55">
-        <v>2.1669</v>
+        <v>2.4597000000000002</v>
       </c>
       <c r="G55">
-        <v>1.4316</v>
+        <v>3.4201000000000001</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
@@ -8832,13 +7920,13 @@
         <v>8</v>
       </c>
       <c r="E56">
-        <v>48.705500000000001</v>
+        <v>51.5535</v>
       </c>
       <c r="F56">
-        <v>4.7560000000000002</v>
+        <v>4.5739000000000001</v>
       </c>
       <c r="G56">
-        <v>4.3249000000000004</v>
+        <v>4.3522999999999996</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
@@ -8855,13 +7943,13 @@
         <v>16</v>
       </c>
       <c r="E57">
-        <v>72.539299999999997</v>
+        <v>74.547899999999998</v>
       </c>
       <c r="F57">
-        <v>17.0229</v>
+        <v>6.7464000000000004</v>
       </c>
       <c r="G57">
-        <v>1.2551000000000001</v>
+        <v>2.0857999999999999</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
@@ -8878,13 +7966,13 @@
         <v>32</v>
       </c>
       <c r="E58">
-        <v>86.202799999999996</v>
+        <v>86.941999999999993</v>
       </c>
       <c r="F58">
-        <v>9.2751999999999999</v>
+        <v>5.3590999999999998</v>
       </c>
       <c r="G58">
-        <v>0.87709999999999999</v>
+        <v>0.28520000000000001</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
@@ -8901,13 +7989,13 @@
         <v>2</v>
       </c>
       <c r="E60">
-        <v>0.58660000000000001</v>
+        <v>0.54069999999999996</v>
       </c>
       <c r="F60">
-        <v>0.47760000000000002</v>
+        <v>0.25580000000000003</v>
       </c>
       <c r="G60">
-        <v>3.4200000000000001E-2</v>
+        <v>0.1242</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
@@ -8924,13 +8012,13 @@
         <v>4</v>
       </c>
       <c r="E61">
-        <v>12.847300000000001</v>
+        <v>8.4076000000000004</v>
       </c>
       <c r="F61">
-        <v>1.9991000000000001</v>
+        <v>1.0987</v>
       </c>
       <c r="G61">
-        <v>0.96419999999999995</v>
+        <v>0.40029999999999999</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
@@ -8947,13 +8035,13 @@
         <v>8</v>
       </c>
       <c r="E62">
-        <v>9.0357000000000003</v>
+        <v>20.292899999999999</v>
       </c>
       <c r="F62">
-        <v>1.6714</v>
+        <v>1.2093</v>
       </c>
       <c r="G62">
-        <v>1.3593</v>
+        <v>1.2435</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
@@ -8970,13 +8058,13 @@
         <v>16</v>
       </c>
       <c r="E63">
-        <v>45.305599999999998</v>
+        <v>48.5443</v>
       </c>
       <c r="F63">
-        <v>9.3844999999999992</v>
+        <v>57.674999999999997</v>
       </c>
       <c r="G63">
-        <v>6.5768000000000004</v>
+        <v>5.8076999999999996</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
@@ -8993,13 +8081,13 @@
         <v>32</v>
       </c>
       <c r="E64">
-        <v>70.626800000000003</v>
+        <v>70.868899999999996</v>
       </c>
       <c r="F64">
-        <v>15.7714</v>
+        <v>2.5278</v>
       </c>
       <c r="G64">
-        <v>4.4715999999999996</v>
+        <v>3.8603000000000001</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
@@ -9022,7 +8110,7 @@
         <v>0</v>
       </c>
       <c r="G66">
-        <v>0.1704</v>
+        <v>0.16450000000000001</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
@@ -9039,13 +8127,13 @@
         <v>4</v>
       </c>
       <c r="E67">
-        <v>0.35759999999999997</v>
+        <v>0.32279999999999998</v>
       </c>
       <c r="F67">
-        <v>0.1701</v>
+        <v>0.1704</v>
       </c>
       <c r="G67">
-        <v>0.25940000000000002</v>
+        <v>0.30659999999999998</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
@@ -9062,13 +8150,13 @@
         <v>8</v>
       </c>
       <c r="E68">
-        <v>12.056800000000001</v>
+        <v>7.8326000000000002</v>
       </c>
       <c r="F68">
-        <v>0.9778</v>
+        <v>0.53480000000000005</v>
       </c>
       <c r="G68">
-        <v>1.0414000000000001</v>
+        <v>0.59230000000000005</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
@@ -9085,13 +8173,13 @@
         <v>16</v>
       </c>
       <c r="E69">
-        <v>8.3058999999999994</v>
+        <v>19.108899999999998</v>
       </c>
       <c r="F69">
-        <v>53.578499999999998</v>
+        <v>9.5305999999999997</v>
       </c>
       <c r="G69">
-        <v>36.668399999999998</v>
+        <v>5.2431999999999999</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
@@ -9108,13 +8196,13 @@
         <v>32</v>
       </c>
       <c r="E70">
-        <v>46.2134</v>
+        <v>49.134099999999997</v>
       </c>
       <c r="F70">
-        <v>22.180199999999999</v>
+        <v>7.6048999999999998</v>
       </c>
       <c r="G70">
-        <v>1.3361000000000001</v>
+        <v>14.9735</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
@@ -9137,7 +8225,7 @@
         <v>0</v>
       </c>
       <c r="G72">
-        <v>3.1199999999999999E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
@@ -9160,7 +8248,7 @@
         <v>0</v>
       </c>
       <c r="G73">
-        <v>3.7600000000000001E-2</v>
+        <v>3.8199999999999998E-2</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
@@ -9177,13 +8265,13 @@
         <v>8</v>
       </c>
       <c r="E74">
-        <v>0.30299999999999999</v>
+        <v>0.27789999999999998</v>
       </c>
       <c r="F74">
-        <v>0.2031</v>
+        <v>0.126</v>
       </c>
       <c r="G74">
-        <v>8.3500000000000005E-2</v>
+        <v>8.2699999999999996E-2</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
@@ -9200,13 +8288,13 @@
         <v>16</v>
       </c>
       <c r="E75">
-        <v>6.3231999999999999</v>
+        <v>7.4836</v>
       </c>
       <c r="F75">
-        <v>9.3424999999999994</v>
+        <v>10.686400000000001</v>
       </c>
       <c r="G75">
-        <v>11.8713</v>
+        <v>16.9773</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
@@ -9223,13 +8311,13 @@
         <v>32</v>
       </c>
       <c r="E76">
-        <v>9.1639999999999997</v>
+        <v>18.7608</v>
       </c>
       <c r="F76">
-        <v>23.888000000000002</v>
+        <v>52.076500000000003</v>
       </c>
       <c r="G76">
-        <v>8.0533000000000001</v>
+        <v>6.1828000000000003</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
@@ -9257,7 +8345,7 @@
         <v>0</v>
       </c>
       <c r="G79">
-        <v>0</v>
+        <v>2.0199999999999999E-2</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
@@ -9280,7 +8368,7 @@
         <v>0</v>
       </c>
       <c r="G80">
-        <v>3.9342999999999999</v>
+        <v>4.1939000000000002</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
@@ -9297,13 +8385,13 @@
         <v>8</v>
       </c>
       <c r="E81">
-        <v>27.0684</v>
+        <v>28.2545</v>
       </c>
       <c r="F81">
-        <v>7.1654</v>
+        <v>7.4649999999999999</v>
       </c>
       <c r="G81">
-        <v>6.6866000000000003</v>
+        <v>6.9352</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
@@ -9320,13 +8408,13 @@
         <v>16</v>
       </c>
       <c r="E82">
-        <v>53.863199999999999</v>
+        <v>55.698</v>
       </c>
       <c r="F82">
-        <v>29.150099999999998</v>
+        <v>10.506500000000001</v>
       </c>
       <c r="G82">
-        <v>3.5114999999999998</v>
+        <v>4.8254999999999999</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
@@ -9343,13 +8431,13 @@
         <v>32</v>
       </c>
       <c r="E83">
-        <v>74.715500000000006</v>
+        <v>75.672300000000007</v>
       </c>
       <c r="F83">
-        <v>16.910799999999998</v>
+        <v>10.219900000000001</v>
       </c>
       <c r="G83">
-        <v>1.7282</v>
+        <v>0.28170000000000001</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
@@ -9435,13 +8523,13 @@
         <v>16</v>
       </c>
       <c r="E88">
-        <v>23.356300000000001</v>
+        <v>23.943000000000001</v>
       </c>
       <c r="F88">
-        <v>14.005100000000001</v>
+        <v>88.225999999999999</v>
       </c>
       <c r="G88">
-        <v>7.4371999999999998</v>
+        <v>9.1936999999999998</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
@@ -9458,13 +8546,13 @@
         <v>32</v>
       </c>
       <c r="E89">
-        <v>51.194899999999997</v>
+        <v>49.468899999999998</v>
       </c>
       <c r="F89">
-        <v>29.153400000000001</v>
+        <v>4.7500999999999998</v>
       </c>
       <c r="G89">
-        <v>7.5613999999999999</v>
+        <v>6.5884999999999998</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
@@ -9550,13 +8638,13 @@
         <v>16</v>
       </c>
       <c r="E94">
-        <v>-7.3788</v>
+        <v>-0.3306</v>
       </c>
       <c r="F94">
-        <v>52.436900000000001</v>
+        <v>11.869</v>
       </c>
       <c r="G94">
-        <v>48.451999999999998</v>
+        <v>10.624700000000001</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
@@ -9573,13 +8661,13 @@
         <v>32</v>
       </c>
       <c r="E95">
-        <v>21.3918</v>
+        <v>23.9117</v>
       </c>
       <c r="F95">
-        <v>51.322600000000001</v>
+        <v>12.570499999999999</v>
       </c>
       <c r="G95">
-        <v>2.7578999999999998</v>
+        <v>25.548999999999999</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
@@ -9665,13 +8753,13 @@
         <v>16</v>
       </c>
       <c r="E100">
-        <v>0.77359999999999995</v>
+        <v>7.5410000000000004</v>
       </c>
       <c r="F100">
-        <v>12.241099999999999</v>
+        <v>14.009499999999999</v>
       </c>
       <c r="G100">
-        <v>27.724699999999999</v>
+        <v>3.8458999999999999</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
@@ -9688,13 +8776,13 @@
         <v>32</v>
       </c>
       <c r="E101">
-        <v>0.30380000000000001</v>
+        <v>6.7545000000000002</v>
       </c>
       <c r="F101">
-        <v>12.4666</v>
+        <v>17.462900000000001</v>
       </c>
       <c r="G101">
-        <v>17.541399999999999</v>
+        <v>11.9122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>